<commit_message>
Finalisation of Raid Log and Development log
</commit_message>
<xml_diff>
--- a/Project Plan (FINAL).xlsx
+++ b/Project Plan (FINAL).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CC Live Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CC Live Project\cc-live-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D81BA247-D200-4E8B-8B9E-9C03FD957844}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7329B4-3846-41B8-BC01-016F8E174DD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>PROJECT NAME</t>
   </si>
@@ -142,9 +142,6 @@
     <t>22/3/2020</t>
   </si>
   <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
     <t xml:space="preserve">                     3.2.1 Features</t>
   </si>
   <si>
@@ -176,6 +173,15 @@
   </si>
   <si>
     <t xml:space="preserve">                     3.2.1.1 Data Preprocessing and Cleaning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   3.2.1.5 Perform Label Encoding on Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   3.2.1.6 Passing data to various Classifiers and getting performance data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   3.2.1.7 Finalising results and selecting best classifier</t>
   </si>
 </sst>
 </file>
@@ -308,15 +314,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -332,6 +329,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,7 +456,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{96286B35-426F-4539-9E60-BC1ECC609F19}" name="Table3" displayName="Table3" ref="A45:G127" headerRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{96286B35-426F-4539-9E60-BC1ECC609F19}" name="Table3" displayName="Table3" ref="A51:G133" headerRowCount="0" totalsRowShown="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{8B4BBD65-D1B8-4F84-B790-C126A13737DB}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{0A15A389-608D-45A9-94B8-028DD92234D4}" name="Column2"/>
@@ -465,8 +471,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E597BDCD-DED1-420E-AAEB-9ADE25728394}" name="Table2" displayName="Table2" ref="A12:G44" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A12:G44" xr:uid="{6846C16E-5172-4549-85C7-42B8014B06CD}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E597BDCD-DED1-420E-AAEB-9ADE25728394}" name="Table2" displayName="Table2" ref="A12:G50" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A12:G50" xr:uid="{6846C16E-5172-4549-85C7-42B8014B06CD}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -751,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,15 +774,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
@@ -793,11 +799,11 @@
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="21">
+      <c r="E4" s="21"/>
+      <c r="F4" s="18">
         <v>44019</v>
       </c>
     </row>
@@ -808,11 +814,11 @@
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="21">
+      <c r="E5" s="21"/>
+      <c r="F5" s="18">
         <v>44039</v>
       </c>
     </row>
@@ -826,7 +832,7 @@
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>43997</v>
       </c>
     </row>
@@ -834,7 +840,7 @@
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <v>44043</v>
       </c>
     </row>
@@ -868,36 +874,36 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="11"/>
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="14"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="11"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="18" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="19">
+      <c r="C15" s="11"/>
+      <c r="D15" s="16">
         <v>43997</v>
       </c>
-      <c r="E15" s="16">
+      <c r="E15" s="13">
         <v>44013</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="11">
         <f>E15-D15</f>
         <v>16</v>
       </c>
@@ -909,13 +915,13 @@
       <c r="B16" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="16">
         <v>43998</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="13">
         <v>44013</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="11">
         <f>E15-D15</f>
         <v>16</v>
       </c>
@@ -924,17 +930,17 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="11"/>
       <c r="B17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="16">
         <v>43999</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>44013</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="11">
         <f>E15-D15</f>
         <v>16</v>
       </c>
@@ -946,13 +952,13 @@
       <c r="B18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="16">
         <v>44000</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="13">
         <v>44013</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="11">
         <f>E15-D15</f>
         <v>16</v>
       </c>
@@ -961,23 +967,23 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
+      <c r="B20" s="12"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="18">
         <v>44013</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="18">
         <v>44019</v>
       </c>
       <c r="F22">
@@ -992,10 +998,10 @@
       <c r="B23" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="18">
         <v>44013</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="18">
         <v>44020</v>
       </c>
       <c r="F23">
@@ -1010,10 +1016,10 @@
       <c r="B24" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="18">
         <v>44013</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="18">
         <v>44021</v>
       </c>
       <c r="F24">
@@ -1025,15 +1031,15 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="17" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D28" s="21">
+      <c r="D28" s="18">
         <v>44013</v>
       </c>
       <c r="E28" t="s">
@@ -1047,7 +1053,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="17" t="s">
         <v>33</v>
       </c>
       <c r="D29" t="s">
@@ -1060,18 +1066,18 @@
         <v>59</v>
       </c>
       <c r="G29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>37</v>
       </c>
       <c r="D30" t="s">
         <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30">
         <v>9</v>
@@ -1079,234 +1085,300 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>47</v>
-      </c>
-      <c r="E32" s="21">
+        <v>46</v>
+      </c>
+      <c r="E32" s="18">
         <v>44019</v>
       </c>
       <c r="F32">
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="20"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="17"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>44</v>
-      </c>
-      <c r="E34" s="21">
+        <v>43</v>
+      </c>
+      <c r="E34" s="18">
         <v>44025</v>
       </c>
       <c r="F34">
         <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E35" s="21"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="E36" s="21">
+        <v>44</v>
+      </c>
+      <c r="E36" s="18">
         <v>44032</v>
       </c>
       <c r="F36">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E37" s="21"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="21">
+        <v>45</v>
+      </c>
+      <c r="E38" s="18">
         <v>44037</v>
       </c>
       <c r="F38">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="21">
-        <v>44037</v>
-      </c>
-      <c r="E40" s="21">
-        <v>44043</v>
+      <c r="G38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E39" s="18"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="18">
+        <v>44038</v>
       </c>
       <c r="F40">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E41" s="18"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="21">
-        <v>44043</v>
-      </c>
-      <c r="E44" s="21">
-        <v>44043</v>
+        <v>48</v>
+      </c>
+      <c r="E42" s="18">
+        <v>44040</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="E43" s="18"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+      <c r="E44" s="18">
+        <v>44041</v>
       </c>
       <c r="F44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="9"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B48" s="7"/>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
+      <c r="G44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" s="18">
+        <v>44037</v>
+      </c>
+      <c r="E46" s="18">
+        <v>44043</v>
+      </c>
+      <c r="F46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="G47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="18">
+        <v>44043</v>
+      </c>
+      <c r="E50" s="18">
+        <v>44043</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
-      <c r="C51" s="9"/>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
     </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
       <c r="B53" s="7"/>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
     </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
     </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B56" s="6"/>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="7"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="5"/>
       <c r="B57" s="7"/>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="5"/>
+    <row r="59" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
-      <c r="C59" s="9"/>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="5"/>
-      <c r="B60" s="6"/>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B61" s="6"/>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="7"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="6"/>
     </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B63" s="6"/>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B64" s="6"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
-    </row>
-    <row r="66" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B66" s="7"/>
-      <c r="C66" s="9"/>
-    </row>
-    <row r="67" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B67" s="7"/>
-    </row>
-    <row r="68" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="7"/>
-    </row>
-    <row r="69" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B69" s="7"/>
-    </row>
-    <row r="70" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B70" s="7"/>
-    </row>
-    <row r="71" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B71" s="7"/>
-    </row>
-    <row r="72" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="7"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="7"/>
+    </row>
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="9"/>
+    </row>
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="6"/>
+    </row>
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B67" s="6"/>
+    </row>
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B68" s="6"/>
+    </row>
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B69" s="6"/>
+    </row>
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B70" s="6"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+    </row>
+    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B72" s="7"/>
-    </row>
-    <row r="73" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C72" s="9"/>
+    </row>
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B73" s="7"/>
     </row>
-    <row r="74" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B74" s="7"/>
     </row>
-    <row r="75" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B75" s="7"/>
     </row>
-    <row r="76" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B76" s="7"/>
-      <c r="C76" s="9"/>
-    </row>
-    <row r="77" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B77" s="7"/>
     </row>
-    <row r="78" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B78" s="7"/>
     </row>
-    <row r="79" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B79" s="7"/>
     </row>
-    <row r="80" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B80" s="7"/>
     </row>
-    <row r="81" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B81" s="7"/>
     </row>
-    <row r="82" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B82" s="7"/>
-    </row>
-    <row r="83" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C82" s="9"/>
+    </row>
+    <row r="83" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B83" s="7"/>
     </row>
-    <row r="84" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B84" s="7"/>
+    </row>
+    <row r="85" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B85" s="7"/>
+    </row>
+    <row r="86" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B86" s="7"/>
+    </row>
+    <row r="87" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B87" s="7"/>
+    </row>
+    <row r="88" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B88" s="7"/>
+    </row>
+    <row r="89" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B89" s="7"/>
+    </row>
+    <row r="90" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B90" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1315,7 +1387,7 @@
     <mergeCell ref="D5:E5"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="G12:G44">
+  <conditionalFormatting sqref="G12:G50">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"COMPLETED"</formula>
     </cfRule>
@@ -1327,7 +1399,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12:G44" xr:uid="{FCD92254-044E-4371-8913-F6D08C76A7CE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G12:G50" xr:uid="{FCD92254-044E-4371-8913-F6D08C76A7CE}">
       <formula1>"IN PROGRESS, PAUSED, COMPLETED"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>